<commit_message>
adding LeftNav_Test code to my fork for troubleshooting the selector issue
</commit_message>
<xml_diff>
--- a/test-data/site-navigation-data.xlsx
+++ b/test-data/site-navigation-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/popkhadzeg/eclipse-workspace/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94BA0E1-6B31-AD4C-90D9-054087486D1C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6404F757-829F-3A43-B530-D6CCD2AB4060}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="3880" windowWidth="28800" windowHeight="16140" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
+    <workbookView xWindow="4800" yWindow="2240" windowWidth="28800" windowHeight="17540" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_site_navigation" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>path</t>
   </si>
@@ -39,27 +39,15 @@
     <t>English</t>
   </si>
   <si>
-    <t>Press Release</t>
-  </si>
-  <si>
     <t>parent</t>
   </si>
   <si>
-    <t>menu</t>
-  </si>
-  <si>
     <t>Feelings and Cancer</t>
   </si>
   <si>
     <t>COPING WITH CANCER</t>
   </si>
   <si>
-    <t>about-cancer/coping</t>
-  </si>
-  <si>
-    <t>ABOUT CANCER</t>
-  </si>
-  <si>
     <t>Learning to Relax</t>
   </si>
   <si>
@@ -67,6 +55,12 @@
   </si>
   <si>
     <t>level2</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>/about-cancer/coping/feelings</t>
   </si>
 </sst>
 </file>
@@ -428,25 +422,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559EFC9A-164C-8144-9EB0-75C1F6F01408}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,39 +450,33 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>